<commit_message>
auto count order and excell generatie
abc me pro
</commit_message>
<xml_diff>
--- a/formatexcel.xlsx
+++ b/formatexcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\FYP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F712EFD7-578E-471D-847F-4792B5E2E547}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE70D25-79EE-4561-A7DB-DDFF72AC113A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{21832C7A-FE32-4B93-8F16-7397E18D770D}"/>
   </bookViews>
@@ -312,7 +312,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -421,18 +421,6 @@
     <font>
       <b/>
       <sz val="18"/>
-      <color rgb="FFFF0000"/>
-      <name val="Century Gothic"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Century Gothic"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Century Gothic"/>
       <family val="2"/>
@@ -663,7 +651,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -681,7 +669,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -715,36 +702,20 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -780,7 +751,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -803,16 +773,42 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -833,10 +829,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -872,10 +868,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -884,12 +877,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -908,9 +895,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -929,10 +913,7 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -959,11 +940,23 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -980,6 +973,9 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="12" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1007,11 +1003,11 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="12" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1025,26 +1021,8 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1082,13 +1060,14 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1253,22 +1232,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>281940</xdr:colOff>
+      <xdr:colOff>384077</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>13774</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>619182</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>175618</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Rectangle 3">
+        <xdr:cNvPr id="5" name="Rectangle 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EC47589-E12E-4F9E-965F-BEA9E7115E6B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2C449C0-19D5-401D-A732-5C521B965134}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1276,8 +1255,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7246620" y="901065"/>
-          <a:ext cx="337242" cy="166093"/>
+          <a:off x="7347585" y="1174359"/>
+          <a:ext cx="348615" cy="185518"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1306,7 +1285,12 @@
         <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
         <a:lstStyle/>
         <a:p>
-          <a:endParaRPr lang="en-US"/>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="ms-MY" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1614,8 +1598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75980BA0-2244-437B-AE4D-E57234A9F6AA}">
   <dimension ref="A1:Y54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Y16" sqref="Y16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="V32" sqref="V32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1651,112 +1635,112 @@
       </c>
     </row>
     <row r="2" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="152"/>
-      <c r="B2" s="152"/>
-      <c r="C2" s="152"/>
-      <c r="D2" s="152"/>
-      <c r="E2" s="152"/>
-      <c r="F2" s="152"/>
-      <c r="G2" s="152"/>
-      <c r="H2" s="152"/>
-      <c r="I2" s="152"/>
-      <c r="J2" s="152"/>
-      <c r="K2" s="152"/>
-      <c r="L2" s="152"/>
-      <c r="M2" s="152"/>
-      <c r="N2" s="152"/>
-      <c r="O2" s="153"/>
-      <c r="P2" s="153"/>
-      <c r="Q2" s="153"/>
-      <c r="R2" s="153"/>
-      <c r="S2" s="153"/>
+      <c r="A2" s="146"/>
+      <c r="B2" s="146"/>
+      <c r="C2" s="146"/>
+      <c r="D2" s="146"/>
+      <c r="E2" s="146"/>
+      <c r="F2" s="146"/>
+      <c r="G2" s="146"/>
+      <c r="H2" s="146"/>
+      <c r="I2" s="146"/>
+      <c r="J2" s="146"/>
+      <c r="K2" s="146"/>
+      <c r="L2" s="146"/>
+      <c r="M2" s="146"/>
+      <c r="N2" s="146"/>
+      <c r="O2" s="147"/>
+      <c r="P2" s="147"/>
+      <c r="Q2" s="147"/>
+      <c r="R2" s="147"/>
+      <c r="S2" s="147"/>
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
     </row>
     <row r="3" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="152" t="s">
+      <c r="A3" s="146" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="152"/>
-      <c r="C3" s="152"/>
-      <c r="D3" s="152"/>
-      <c r="E3" s="152"/>
-      <c r="F3" s="152"/>
-      <c r="G3" s="152"/>
-      <c r="H3" s="152"/>
-      <c r="I3" s="152"/>
-      <c r="J3" s="152"/>
-      <c r="K3" s="152"/>
-      <c r="L3" s="152"/>
-      <c r="M3" s="152"/>
-      <c r="N3" s="152"/>
-      <c r="O3" s="152"/>
-      <c r="P3" s="152"/>
-      <c r="Q3" s="152"/>
-      <c r="R3" s="152"/>
-      <c r="S3" s="152"/>
-      <c r="T3" s="152"/>
-      <c r="U3" s="152"/>
-      <c r="V3" s="152"/>
+      <c r="B3" s="146"/>
+      <c r="C3" s="146"/>
+      <c r="D3" s="146"/>
+      <c r="E3" s="146"/>
+      <c r="F3" s="146"/>
+      <c r="G3" s="146"/>
+      <c r="H3" s="146"/>
+      <c r="I3" s="146"/>
+      <c r="J3" s="146"/>
+      <c r="K3" s="146"/>
+      <c r="L3" s="146"/>
+      <c r="M3" s="146"/>
+      <c r="N3" s="146"/>
+      <c r="O3" s="146"/>
+      <c r="P3" s="146"/>
+      <c r="Q3" s="146"/>
+      <c r="R3" s="146"/>
+      <c r="S3" s="146"/>
+      <c r="T3" s="146"/>
+      <c r="U3" s="146"/>
+      <c r="V3" s="146"/>
     </row>
     <row r="4" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="152" t="s">
+      <c r="A4" s="146" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="152"/>
-      <c r="C4" s="152"/>
-      <c r="D4" s="152"/>
-      <c r="E4" s="152"/>
-      <c r="F4" s="152"/>
-      <c r="G4" s="152"/>
-      <c r="H4" s="152"/>
-      <c r="I4" s="152"/>
-      <c r="J4" s="152"/>
-      <c r="K4" s="152"/>
-      <c r="L4" s="152"/>
-      <c r="M4" s="152"/>
-      <c r="N4" s="152"/>
-      <c r="O4" s="152"/>
-      <c r="P4" s="152"/>
-      <c r="Q4" s="152"/>
-      <c r="R4" s="152"/>
-      <c r="S4" s="152"/>
-      <c r="T4" s="152"/>
-      <c r="U4" s="152"/>
-      <c r="V4" s="152"/>
-      <c r="W4" s="156"/>
-      <c r="X4" s="157"/>
-      <c r="Y4" s="157"/>
+      <c r="B4" s="146"/>
+      <c r="C4" s="146"/>
+      <c r="D4" s="146"/>
+      <c r="E4" s="146"/>
+      <c r="F4" s="146"/>
+      <c r="G4" s="146"/>
+      <c r="H4" s="146"/>
+      <c r="I4" s="146"/>
+      <c r="J4" s="146"/>
+      <c r="K4" s="146"/>
+      <c r="L4" s="146"/>
+      <c r="M4" s="146"/>
+      <c r="N4" s="146"/>
+      <c r="O4" s="146"/>
+      <c r="P4" s="146"/>
+      <c r="Q4" s="146"/>
+      <c r="R4" s="146"/>
+      <c r="S4" s="146"/>
+      <c r="T4" s="146"/>
+      <c r="U4" s="146"/>
+      <c r="V4" s="146"/>
+      <c r="W4" s="54"/>
+      <c r="X4" s="55"/>
+      <c r="Y4" s="55"/>
     </row>
     <row r="5" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="152" t="s">
+      <c r="A5" s="146" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="152"/>
-      <c r="C5" s="152"/>
-      <c r="D5" s="152"/>
-      <c r="E5" s="152"/>
-      <c r="F5" s="152"/>
-      <c r="G5" s="152"/>
-      <c r="H5" s="152"/>
-      <c r="I5" s="152"/>
-      <c r="J5" s="152"/>
-      <c r="K5" s="152"/>
-      <c r="L5" s="152"/>
-      <c r="M5" s="152"/>
-      <c r="N5" s="152"/>
-      <c r="O5" s="152"/>
-      <c r="P5" s="152"/>
-      <c r="Q5" s="152"/>
-      <c r="R5" s="152"/>
-      <c r="S5" s="152"/>
-      <c r="T5" s="152"/>
-      <c r="U5" s="152"/>
-      <c r="V5" s="152"/>
-      <c r="W5" s="157"/>
-      <c r="X5" s="157"/>
-      <c r="Y5" s="157"/>
+      <c r="B5" s="146"/>
+      <c r="C5" s="146"/>
+      <c r="D5" s="146"/>
+      <c r="E5" s="146"/>
+      <c r="F5" s="146"/>
+      <c r="G5" s="146"/>
+      <c r="H5" s="146"/>
+      <c r="I5" s="146"/>
+      <c r="J5" s="146"/>
+      <c r="K5" s="146"/>
+      <c r="L5" s="146"/>
+      <c r="M5" s="146"/>
+      <c r="N5" s="146"/>
+      <c r="O5" s="146"/>
+      <c r="P5" s="146"/>
+      <c r="Q5" s="146"/>
+      <c r="R5" s="146"/>
+      <c r="S5" s="146"/>
+      <c r="T5" s="146"/>
+      <c r="U5" s="146"/>
+      <c r="V5" s="146"/>
+      <c r="W5" s="55"/>
+      <c r="X5" s="55"/>
+      <c r="Y5" s="55"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
@@ -1786,573 +1770,573 @@
         <v>4</v>
       </c>
       <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8" t="s">
         <v>5</v>
       </c>
       <c r="K7" s="8"/>
-      <c r="L7" s="10"/>
+      <c r="L7" s="9"/>
       <c r="M7" s="8"/>
-      <c r="N7" s="154"/>
-      <c r="O7" s="155"/>
-      <c r="P7" s="155"/>
-      <c r="Q7" s="155"/>
-      <c r="R7" s="11"/>
+      <c r="N7" s="148"/>
+      <c r="O7" s="149"/>
+      <c r="P7" s="149"/>
+      <c r="Q7" s="149"/>
+      <c r="R7" s="10"/>
       <c r="S7" s="8" t="s">
         <v>6</v>
       </c>
       <c r="T7" s="8"/>
       <c r="U7" s="8"/>
       <c r="V7" s="8"/>
-      <c r="W7" s="12"/>
+      <c r="W7" s="11"/>
     </row>
     <row r="8" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="R8" s="12"/>
-      <c r="S8" s="12"/>
-      <c r="T8" s="12"/>
-      <c r="U8" s="12"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A9" s="144" t="s">
+      <c r="A9" s="138" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="145" t="s">
+      <c r="B9" s="139" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="145"/>
-      <c r="D9" s="145"/>
-      <c r="E9" s="145"/>
-      <c r="F9" s="145" t="s">
+      <c r="C9" s="139"/>
+      <c r="D9" s="139"/>
+      <c r="E9" s="139"/>
+      <c r="F9" s="139" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="145"/>
-      <c r="H9" s="145" t="s">
+      <c r="G9" s="139"/>
+      <c r="H9" s="139" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="145"/>
-      <c r="J9" s="146" t="s">
+      <c r="I9" s="139"/>
+      <c r="J9" s="140" t="s">
         <v>11</v>
       </c>
-      <c r="K9" s="147"/>
-      <c r="L9" s="147"/>
-      <c r="M9" s="148"/>
-      <c r="N9" s="145" t="s">
+      <c r="K9" s="141"/>
+      <c r="L9" s="141"/>
+      <c r="M9" s="142"/>
+      <c r="N9" s="139" t="s">
         <v>12</v>
       </c>
-      <c r="O9" s="145"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="14" t="s">
+      <c r="O9" s="139"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="R9" s="15"/>
-      <c r="S9" s="15"/>
-      <c r="T9" s="15"/>
-      <c r="U9" s="15"/>
-      <c r="V9" s="16" t="s">
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="W9" s="17"/>
+      <c r="W9" s="16"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A10" s="144"/>
-      <c r="B10" s="145"/>
-      <c r="C10" s="145"/>
-      <c r="D10" s="145"/>
-      <c r="E10" s="145"/>
-      <c r="F10" s="145"/>
-      <c r="G10" s="145"/>
-      <c r="H10" s="145"/>
-      <c r="I10" s="145"/>
-      <c r="J10" s="149"/>
-      <c r="K10" s="150"/>
-      <c r="L10" s="150"/>
-      <c r="M10" s="151"/>
-      <c r="N10" s="145"/>
-      <c r="O10" s="145"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="19" t="s">
+      <c r="A10" s="138"/>
+      <c r="B10" s="139"/>
+      <c r="C10" s="139"/>
+      <c r="D10" s="139"/>
+      <c r="E10" s="139"/>
+      <c r="F10" s="139"/>
+      <c r="G10" s="139"/>
+      <c r="H10" s="139"/>
+      <c r="I10" s="139"/>
+      <c r="J10" s="143"/>
+      <c r="K10" s="144"/>
+      <c r="L10" s="144"/>
+      <c r="M10" s="145"/>
+      <c r="N10" s="139"/>
+      <c r="O10" s="139"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="R10" s="20" t="s">
+      <c r="R10" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="S10" s="21" t="s">
+      <c r="S10" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="T10" s="22"/>
-      <c r="U10" s="22"/>
-      <c r="V10" s="23"/>
-      <c r="W10" s="17"/>
+      <c r="T10" s="21"/>
+      <c r="U10" s="21"/>
+      <c r="V10" s="58"/>
+      <c r="W10" s="16"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A11" s="24">
+      <c r="A11" s="22">
         <v>1</v>
       </c>
-      <c r="B11" s="139"/>
-      <c r="C11" s="140"/>
-      <c r="D11" s="140"/>
-      <c r="E11" s="141"/>
-      <c r="F11" s="139"/>
-      <c r="G11" s="141"/>
-      <c r="H11" s="142"/>
-      <c r="I11" s="143"/>
+      <c r="B11" s="150"/>
+      <c r="C11" s="151"/>
+      <c r="D11" s="151"/>
+      <c r="E11" s="152"/>
+      <c r="F11" s="150"/>
+      <c r="G11" s="152"/>
+      <c r="H11" s="150"/>
+      <c r="I11" s="151"/>
       <c r="J11" s="135"/>
       <c r="K11" s="136"/>
       <c r="L11" s="136"/>
-      <c r="M11" s="87"/>
+      <c r="M11" s="137"/>
       <c r="N11" s="135"/>
-      <c r="O11" s="87"/>
-      <c r="Q11" s="19" t="s">
+      <c r="O11" s="137"/>
+      <c r="Q11" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="R11" s="20" t="s">
+      <c r="R11" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="S11" s="21" t="s">
+      <c r="S11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="T11" s="22"/>
-      <c r="U11" s="22"/>
-      <c r="V11" s="20"/>
+      <c r="T11" s="21"/>
+      <c r="U11" s="21"/>
+      <c r="V11" s="58"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A12" s="24">
+      <c r="A12" s="22">
         <v>2</v>
       </c>
       <c r="B12" s="135"/>
       <c r="C12" s="136"/>
       <c r="D12" s="136"/>
-      <c r="E12" s="87"/>
+      <c r="E12" s="137"/>
       <c r="F12" s="135"/>
-      <c r="G12" s="87"/>
-      <c r="H12" s="137"/>
-      <c r="I12" s="138"/>
+      <c r="G12" s="137"/>
+      <c r="H12" s="135"/>
+      <c r="I12" s="136"/>
       <c r="J12" s="135"/>
       <c r="K12" s="136"/>
       <c r="L12" s="136"/>
-      <c r="M12" s="87"/>
+      <c r="M12" s="137"/>
       <c r="N12" s="135"/>
-      <c r="O12" s="87"/>
-      <c r="Q12" s="19" t="s">
+      <c r="O12" s="137"/>
+      <c r="Q12" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="R12" s="20" t="s">
+      <c r="R12" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="S12" s="21" t="s">
+      <c r="S12" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="T12" s="22"/>
-      <c r="U12" s="22"/>
-      <c r="V12" s="20"/>
+      <c r="T12" s="21"/>
+      <c r="U12" s="21"/>
+      <c r="V12" s="58"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A13" s="24">
+      <c r="A13" s="22">
         <v>3</v>
       </c>
       <c r="B13" s="135"/>
       <c r="C13" s="136"/>
       <c r="D13" s="136"/>
-      <c r="E13" s="87"/>
+      <c r="E13" s="137"/>
       <c r="F13" s="135"/>
-      <c r="G13" s="87"/>
-      <c r="H13" s="137"/>
-      <c r="I13" s="138"/>
+      <c r="G13" s="137"/>
+      <c r="H13" s="135"/>
+      <c r="I13" s="136"/>
       <c r="J13" s="135"/>
       <c r="K13" s="136"/>
       <c r="L13" s="136"/>
-      <c r="M13" s="87"/>
+      <c r="M13" s="137"/>
       <c r="N13" s="135"/>
-      <c r="O13" s="87"/>
-      <c r="Q13" s="19" t="s">
+      <c r="O13" s="137"/>
+      <c r="Q13" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="R13" s="20" t="s">
+      <c r="R13" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="S13" s="21" t="s">
+      <c r="S13" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T13" s="22"/>
-      <c r="U13" s="22"/>
-      <c r="V13" s="23"/>
+      <c r="T13" s="21"/>
+      <c r="U13" s="21"/>
+      <c r="V13" s="62"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A14" s="24">
+      <c r="A14" s="22">
         <v>4</v>
       </c>
       <c r="B14" s="135"/>
       <c r="C14" s="136"/>
       <c r="D14" s="136"/>
-      <c r="E14" s="87"/>
+      <c r="E14" s="137"/>
       <c r="F14" s="135"/>
-      <c r="G14" s="87"/>
-      <c r="H14" s="137"/>
-      <c r="I14" s="138"/>
+      <c r="G14" s="137"/>
+      <c r="H14" s="135"/>
+      <c r="I14" s="136"/>
       <c r="J14" s="135"/>
       <c r="K14" s="136"/>
       <c r="L14" s="136"/>
-      <c r="M14" s="87"/>
+      <c r="M14" s="137"/>
       <c r="N14" s="135"/>
-      <c r="O14" s="87"/>
-      <c r="Q14" s="19" t="s">
+      <c r="O14" s="137"/>
+      <c r="Q14" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="R14" s="20" t="s">
+      <c r="R14" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="S14" s="21" t="s">
+      <c r="S14" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="T14" s="22"/>
-      <c r="U14" s="22"/>
-      <c r="V14" s="23"/>
+      <c r="T14" s="21"/>
+      <c r="U14" s="21"/>
+      <c r="V14" s="62"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A15" s="24">
+      <c r="A15" s="22">
         <v>5</v>
       </c>
       <c r="B15" s="135"/>
       <c r="C15" s="136"/>
       <c r="D15" s="136"/>
-      <c r="E15" s="87"/>
+      <c r="E15" s="137"/>
       <c r="F15" s="135"/>
-      <c r="G15" s="87"/>
-      <c r="H15" s="137"/>
-      <c r="I15" s="138"/>
+      <c r="G15" s="137"/>
+      <c r="H15" s="135"/>
+      <c r="I15" s="136"/>
       <c r="J15" s="135"/>
       <c r="K15" s="136"/>
       <c r="L15" s="136"/>
-      <c r="M15" s="87"/>
+      <c r="M15" s="137"/>
       <c r="N15" s="135"/>
-      <c r="O15" s="87"/>
-      <c r="Q15" s="19" t="s">
+      <c r="O15" s="137"/>
+      <c r="Q15" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="R15" s="20" t="s">
+      <c r="R15" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="S15" s="21" t="s">
+      <c r="S15" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="T15" s="22"/>
-      <c r="U15" s="22"/>
-      <c r="V15" s="25"/>
+      <c r="T15" s="21"/>
+      <c r="U15" s="21"/>
+      <c r="V15" s="62"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A16" s="24">
+      <c r="A16" s="22">
         <v>6</v>
       </c>
       <c r="B16" s="75"/>
-      <c r="C16" s="113"/>
-      <c r="D16" s="113"/>
+      <c r="C16" s="108"/>
+      <c r="D16" s="108"/>
       <c r="E16" s="76"/>
       <c r="F16" s="75"/>
       <c r="G16" s="76"/>
       <c r="H16" s="75"/>
-      <c r="I16" s="113"/>
+      <c r="I16" s="108"/>
       <c r="J16" s="75"/>
-      <c r="K16" s="113"/>
-      <c r="L16" s="113"/>
+      <c r="K16" s="108"/>
+      <c r="L16" s="108"/>
       <c r="M16" s="76"/>
       <c r="N16" s="75"/>
       <c r="O16" s="76"/>
-      <c r="Q16" s="19" t="s">
+      <c r="Q16" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="R16" s="20" t="s">
+      <c r="R16" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="S16" s="21" t="s">
+      <c r="S16" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="T16" s="22"/>
-      <c r="U16" s="22"/>
-      <c r="V16" s="25"/>
+      <c r="T16" s="21"/>
+      <c r="U16" s="21"/>
+      <c r="V16" s="62"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A17" s="24">
+      <c r="A17" s="22">
         <v>7</v>
       </c>
       <c r="B17" s="75"/>
-      <c r="C17" s="113"/>
-      <c r="D17" s="113"/>
+      <c r="C17" s="108"/>
+      <c r="D17" s="108"/>
       <c r="E17" s="76"/>
       <c r="F17" s="75"/>
       <c r="G17" s="76"/>
       <c r="H17" s="75"/>
-      <c r="I17" s="113"/>
+      <c r="I17" s="108"/>
       <c r="J17" s="75"/>
-      <c r="K17" s="113"/>
-      <c r="L17" s="113"/>
+      <c r="K17" s="108"/>
+      <c r="L17" s="108"/>
       <c r="M17" s="76"/>
       <c r="N17" s="75"/>
       <c r="O17" s="76"/>
-      <c r="Q17" s="19" t="s">
+      <c r="Q17" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="R17" s="20" t="s">
+      <c r="R17" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="S17" s="21" t="s">
+      <c r="S17" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="T17" s="22"/>
-      <c r="U17" s="22"/>
-      <c r="V17" s="25"/>
+      <c r="T17" s="21"/>
+      <c r="U17" s="21"/>
+      <c r="V17" s="62"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A18" s="24">
+      <c r="A18" s="22">
         <v>8</v>
       </c>
       <c r="B18" s="75"/>
-      <c r="C18" s="113"/>
-      <c r="D18" s="113"/>
+      <c r="C18" s="108"/>
+      <c r="D18" s="108"/>
       <c r="E18" s="76"/>
       <c r="F18" s="75"/>
       <c r="G18" s="76"/>
       <c r="H18" s="75"/>
-      <c r="I18" s="113"/>
+      <c r="I18" s="108"/>
       <c r="J18" s="75"/>
-      <c r="K18" s="113"/>
-      <c r="L18" s="113"/>
+      <c r="K18" s="108"/>
+      <c r="L18" s="108"/>
       <c r="M18" s="76"/>
       <c r="N18" s="75"/>
       <c r="O18" s="76"/>
-      <c r="Q18" s="19" t="s">
+      <c r="Q18" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="R18" s="20" t="s">
+      <c r="R18" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="S18" s="26" t="s">
+      <c r="S18" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="T18" s="27"/>
-      <c r="U18" s="27"/>
-      <c r="V18" s="28"/>
+      <c r="T18" s="24"/>
+      <c r="U18" s="24"/>
+      <c r="V18" s="62"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A19" s="24">
+      <c r="A19" s="22">
         <v>9</v>
       </c>
       <c r="B19" s="75"/>
-      <c r="C19" s="113"/>
-      <c r="D19" s="113"/>
+      <c r="C19" s="108"/>
+      <c r="D19" s="108"/>
       <c r="E19" s="76"/>
       <c r="F19" s="75"/>
       <c r="G19" s="76"/>
       <c r="H19" s="75"/>
-      <c r="I19" s="113"/>
+      <c r="I19" s="108"/>
       <c r="J19" s="75"/>
-      <c r="K19" s="113"/>
-      <c r="L19" s="113"/>
+      <c r="K19" s="108"/>
+      <c r="L19" s="108"/>
       <c r="M19" s="76"/>
       <c r="N19" s="75"/>
       <c r="O19" s="76"/>
-      <c r="Q19" s="19" t="s">
+      <c r="Q19" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="R19" s="20" t="s">
+      <c r="R19" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="S19" s="26" t="s">
+      <c r="S19" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="T19" s="27"/>
-      <c r="U19" s="27"/>
-      <c r="V19" s="28"/>
+      <c r="T19" s="24"/>
+      <c r="U19" s="24"/>
+      <c r="V19" s="62"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A20" s="24">
+      <c r="A20" s="22">
         <v>10</v>
       </c>
       <c r="B20" s="75"/>
-      <c r="C20" s="113"/>
-      <c r="D20" s="113"/>
+      <c r="C20" s="108"/>
+      <c r="D20" s="108"/>
       <c r="E20" s="76"/>
       <c r="F20" s="75"/>
       <c r="G20" s="76"/>
       <c r="H20" s="75"/>
-      <c r="I20" s="113"/>
+      <c r="I20" s="108"/>
       <c r="J20" s="75"/>
-      <c r="K20" s="113"/>
-      <c r="L20" s="113"/>
+      <c r="K20" s="108"/>
+      <c r="L20" s="108"/>
       <c r="M20" s="76"/>
       <c r="N20" s="75"/>
       <c r="O20" s="76"/>
-      <c r="Q20" s="19" t="s">
+      <c r="Q20" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="R20" s="20" t="s">
+      <c r="R20" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="S20" s="21" t="s">
+      <c r="S20" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="T20" s="22"/>
-      <c r="U20" s="22"/>
-      <c r="V20" s="25"/>
+      <c r="T20" s="21"/>
+      <c r="U20" s="21"/>
+      <c r="V20" s="62"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A21" s="24">
+      <c r="A21" s="22">
         <v>11</v>
       </c>
       <c r="B21" s="75"/>
-      <c r="C21" s="113"/>
-      <c r="D21" s="113"/>
+      <c r="C21" s="108"/>
+      <c r="D21" s="108"/>
       <c r="E21" s="76"/>
       <c r="F21" s="75"/>
       <c r="G21" s="76"/>
       <c r="H21" s="75"/>
       <c r="I21" s="76"/>
       <c r="J21" s="75"/>
-      <c r="K21" s="113"/>
-      <c r="L21" s="113"/>
+      <c r="K21" s="108"/>
+      <c r="L21" s="108"/>
       <c r="M21" s="76"/>
       <c r="N21" s="75"/>
       <c r="O21" s="76"/>
-      <c r="Q21" s="19" t="s">
+      <c r="Q21" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="R21" s="20" t="s">
+      <c r="R21" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="S21" s="21" t="s">
+      <c r="S21" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="T21" s="22"/>
-      <c r="U21" s="22"/>
-      <c r="V21" s="25"/>
+      <c r="T21" s="21"/>
+      <c r="U21" s="21"/>
+      <c r="V21" s="62"/>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A22" s="24">
+      <c r="A22" s="22">
         <v>12</v>
       </c>
       <c r="B22" s="75"/>
-      <c r="C22" s="113"/>
-      <c r="D22" s="113"/>
+      <c r="C22" s="108"/>
+      <c r="D22" s="108"/>
       <c r="E22" s="76"/>
       <c r="F22" s="75"/>
       <c r="G22" s="76"/>
       <c r="H22" s="75"/>
       <c r="I22" s="76"/>
       <c r="J22" s="75"/>
-      <c r="K22" s="113"/>
-      <c r="L22" s="113"/>
+      <c r="K22" s="108"/>
+      <c r="L22" s="108"/>
       <c r="M22" s="76"/>
       <c r="N22" s="75"/>
       <c r="O22" s="76"/>
-      <c r="Q22" s="19" t="s">
+      <c r="Q22" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="R22" s="20" t="s">
+      <c r="R22" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="S22" s="21" t="s">
+      <c r="S22" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="T22" s="22"/>
-      <c r="U22" s="22"/>
-      <c r="V22" s="25"/>
+      <c r="T22" s="21"/>
+      <c r="U22" s="21"/>
+      <c r="V22" s="62"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A23" s="24">
+      <c r="A23" s="22">
         <v>13</v>
       </c>
       <c r="B23" s="75"/>
-      <c r="C23" s="113"/>
-      <c r="D23" s="113"/>
+      <c r="C23" s="108"/>
+      <c r="D23" s="108"/>
       <c r="E23" s="76"/>
       <c r="F23" s="75"/>
       <c r="G23" s="76"/>
       <c r="H23" s="75"/>
       <c r="I23" s="76"/>
       <c r="J23" s="75"/>
-      <c r="K23" s="113"/>
-      <c r="L23" s="113"/>
+      <c r="K23" s="108"/>
+      <c r="L23" s="108"/>
       <c r="M23" s="76"/>
       <c r="N23" s="75"/>
       <c r="O23" s="76"/>
-      <c r="Q23" s="19" t="s">
+      <c r="Q23" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="R23" s="20" t="s">
+      <c r="R23" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="S23" s="21" t="s">
+      <c r="S23" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="T23" s="22"/>
-      <c r="U23" s="22"/>
-      <c r="V23" s="25"/>
+      <c r="T23" s="21"/>
+      <c r="U23" s="21"/>
+      <c r="V23" s="62"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A24" s="24">
+      <c r="A24" s="22">
         <v>14</v>
       </c>
       <c r="B24" s="75"/>
-      <c r="C24" s="113"/>
-      <c r="D24" s="113"/>
+      <c r="C24" s="108"/>
+      <c r="D24" s="108"/>
       <c r="E24" s="76"/>
       <c r="F24" s="75"/>
       <c r="G24" s="76"/>
       <c r="H24" s="75"/>
       <c r="I24" s="76"/>
       <c r="J24" s="75"/>
-      <c r="K24" s="113"/>
-      <c r="L24" s="113"/>
+      <c r="K24" s="108"/>
+      <c r="L24" s="108"/>
       <c r="M24" s="76"/>
       <c r="N24" s="75"/>
       <c r="O24" s="76"/>
-      <c r="Q24" s="19" t="s">
+      <c r="Q24" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="R24" s="20" t="s">
+      <c r="R24" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="S24" s="21" t="s">
+      <c r="S24" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="T24" s="22"/>
-      <c r="U24" s="22"/>
-      <c r="V24" s="25"/>
+      <c r="T24" s="21"/>
+      <c r="U24" s="21"/>
+      <c r="V24" s="62"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A25" s="24">
+      <c r="A25" s="22">
         <v>15</v>
       </c>
       <c r="B25" s="75"/>
-      <c r="C25" s="113"/>
-      <c r="D25" s="113"/>
+      <c r="C25" s="108"/>
+      <c r="D25" s="108"/>
       <c r="E25" s="76"/>
       <c r="F25" s="75"/>
       <c r="G25" s="76"/>
       <c r="H25" s="75"/>
       <c r="I25" s="76"/>
       <c r="J25" s="75"/>
-      <c r="K25" s="113"/>
-      <c r="L25" s="113"/>
+      <c r="K25" s="108"/>
+      <c r="L25" s="108"/>
       <c r="M25" s="76"/>
       <c r="N25" s="75"/>
       <c r="O25" s="76"/>
@@ -2370,20 +2354,20 @@
       <c r="V25" s="131"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A26" s="24">
+      <c r="A26" s="22">
         <v>16</v>
       </c>
       <c r="B26" s="75"/>
-      <c r="C26" s="113"/>
-      <c r="D26" s="113"/>
+      <c r="C26" s="108"/>
+      <c r="D26" s="108"/>
       <c r="E26" s="76"/>
       <c r="F26" s="75"/>
       <c r="G26" s="76"/>
       <c r="H26" s="75"/>
       <c r="I26" s="76"/>
       <c r="J26" s="75"/>
-      <c r="K26" s="113"/>
-      <c r="L26" s="113"/>
+      <c r="K26" s="108"/>
+      <c r="L26" s="108"/>
       <c r="M26" s="76"/>
       <c r="N26" s="75"/>
       <c r="O26" s="76"/>
@@ -2395,488 +2379,491 @@
       <c r="V26" s="132"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A27" s="24">
+      <c r="A27" s="22">
         <v>17</v>
       </c>
       <c r="B27" s="75"/>
-      <c r="C27" s="113"/>
-      <c r="D27" s="113"/>
+      <c r="C27" s="108"/>
+      <c r="D27" s="108"/>
       <c r="E27" s="76"/>
       <c r="F27" s="75"/>
       <c r="G27" s="76"/>
       <c r="H27" s="75"/>
       <c r="I27" s="76"/>
       <c r="J27" s="75"/>
-      <c r="K27" s="113"/>
-      <c r="L27" s="113"/>
+      <c r="K27" s="108"/>
+      <c r="L27" s="108"/>
       <c r="M27" s="76"/>
       <c r="N27" s="75"/>
       <c r="O27" s="76"/>
       <c r="Q27" s="122">
         <v>17</v>
       </c>
-      <c r="R27" s="120" t="s">
+      <c r="R27" s="119" t="s">
         <v>63</v>
       </c>
-      <c r="S27" s="121" t="s">
+      <c r="S27" s="120" t="s">
         <v>64</v>
       </c>
-      <c r="T27" s="121"/>
-      <c r="U27" s="121"/>
-      <c r="V27" s="120"/>
+      <c r="T27" s="120"/>
+      <c r="U27" s="120"/>
+      <c r="V27" s="121"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A28" s="24">
+      <c r="A28" s="22">
         <v>18</v>
       </c>
       <c r="B28" s="75"/>
-      <c r="C28" s="113"/>
-      <c r="D28" s="113"/>
+      <c r="C28" s="108"/>
+      <c r="D28" s="108"/>
       <c r="E28" s="76"/>
       <c r="F28" s="75"/>
       <c r="G28" s="76"/>
       <c r="H28" s="75"/>
       <c r="I28" s="76"/>
       <c r="J28" s="75"/>
-      <c r="K28" s="113"/>
-      <c r="L28" s="113"/>
+      <c r="K28" s="108"/>
+      <c r="L28" s="108"/>
       <c r="M28" s="76"/>
       <c r="N28" s="75"/>
       <c r="O28" s="76"/>
       <c r="Q28" s="122"/>
-      <c r="R28" s="120"/>
-      <c r="S28" s="121"/>
-      <c r="T28" s="121"/>
-      <c r="U28" s="121"/>
-      <c r="V28" s="120"/>
+      <c r="R28" s="119"/>
+      <c r="S28" s="120"/>
+      <c r="T28" s="120"/>
+      <c r="U28" s="120"/>
+      <c r="V28" s="121"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A29" s="24">
+      <c r="A29" s="22">
         <v>19</v>
       </c>
       <c r="B29" s="75"/>
-      <c r="C29" s="113"/>
-      <c r="D29" s="113"/>
+      <c r="C29" s="108"/>
+      <c r="D29" s="108"/>
       <c r="E29" s="76"/>
       <c r="F29" s="75"/>
       <c r="G29" s="76"/>
       <c r="H29" s="75"/>
       <c r="I29" s="76"/>
       <c r="J29" s="75"/>
-      <c r="K29" s="113"/>
-      <c r="L29" s="113"/>
+      <c r="K29" s="108"/>
+      <c r="L29" s="108"/>
       <c r="M29" s="76"/>
       <c r="N29" s="75"/>
       <c r="O29" s="76"/>
-      <c r="Q29" s="29">
+      <c r="Q29" s="25">
         <v>18</v>
       </c>
-      <c r="R29" s="30" t="s">
+      <c r="R29" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="S29" s="117" t="s">
+      <c r="S29" s="116" t="s">
         <v>66</v>
       </c>
-      <c r="T29" s="118"/>
-      <c r="U29" s="119"/>
-      <c r="V29" s="31"/>
+      <c r="T29" s="117"/>
+      <c r="U29" s="118"/>
+      <c r="V29" s="62"/>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A30" s="24">
+      <c r="A30" s="22">
         <v>20</v>
       </c>
       <c r="B30" s="75"/>
-      <c r="C30" s="113"/>
-      <c r="D30" s="113"/>
+      <c r="C30" s="108"/>
+      <c r="D30" s="108"/>
       <c r="E30" s="76"/>
       <c r="F30" s="75"/>
       <c r="G30" s="76"/>
       <c r="H30" s="75"/>
       <c r="I30" s="76"/>
       <c r="J30" s="75"/>
-      <c r="K30" s="113"/>
-      <c r="L30" s="113"/>
+      <c r="K30" s="108"/>
+      <c r="L30" s="108"/>
       <c r="M30" s="76"/>
       <c r="N30" s="75"/>
       <c r="O30" s="76"/>
-      <c r="Q30" s="29">
+      <c r="Q30" s="25">
         <v>19</v>
       </c>
-      <c r="R30" s="30" t="s">
+      <c r="R30" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="S30" s="117" t="s">
+      <c r="S30" s="116" t="s">
         <v>87</v>
       </c>
-      <c r="T30" s="118"/>
-      <c r="U30" s="119"/>
-      <c r="V30" s="31"/>
+      <c r="T30" s="117"/>
+      <c r="U30" s="118"/>
+      <c r="V30" s="62"/>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A31" s="24">
+      <c r="A31" s="22">
         <v>21</v>
       </c>
       <c r="B31" s="75"/>
-      <c r="C31" s="113"/>
-      <c r="D31" s="113"/>
+      <c r="C31" s="108"/>
+      <c r="D31" s="108"/>
       <c r="E31" s="76"/>
       <c r="F31" s="75"/>
       <c r="G31" s="76"/>
       <c r="H31" s="75"/>
       <c r="I31" s="76"/>
       <c r="J31" s="75"/>
-      <c r="K31" s="113"/>
-      <c r="L31" s="113"/>
+      <c r="K31" s="108"/>
+      <c r="L31" s="108"/>
       <c r="M31" s="76"/>
       <c r="N31" s="75"/>
       <c r="O31" s="76"/>
-      <c r="Q31" s="25"/>
-      <c r="R31" s="25"/>
-      <c r="S31" s="116"/>
-      <c r="T31" s="116"/>
-      <c r="U31" s="116"/>
-      <c r="V31" s="32"/>
+      <c r="Q31" s="62"/>
+      <c r="R31" s="62"/>
+      <c r="S31" s="110"/>
+      <c r="T31" s="111"/>
+      <c r="U31" s="112"/>
+      <c r="V31" s="62"/>
     </row>
     <row r="32" spans="1:22" ht="23.4" x14ac:dyDescent="0.4">
-      <c r="A32" s="24">
+      <c r="A32" s="22">
         <v>22</v>
       </c>
       <c r="B32" s="75"/>
-      <c r="C32" s="113"/>
-      <c r="D32" s="113"/>
+      <c r="C32" s="108"/>
+      <c r="D32" s="108"/>
       <c r="E32" s="76"/>
       <c r="F32" s="75"/>
       <c r="G32" s="76"/>
       <c r="H32" s="75"/>
       <c r="I32" s="76"/>
       <c r="J32" s="75"/>
-      <c r="K32" s="113"/>
-      <c r="L32" s="113"/>
+      <c r="K32" s="108"/>
+      <c r="L32" s="108"/>
       <c r="M32" s="76"/>
       <c r="N32" s="75"/>
       <c r="O32" s="76"/>
-      <c r="Q32" s="115" t="s">
+      <c r="Q32" s="113" t="s">
         <v>67</v>
       </c>
-      <c r="R32" s="158"/>
-      <c r="S32" s="158"/>
-      <c r="T32" s="158"/>
-      <c r="U32" s="159"/>
-      <c r="V32" s="33"/>
+      <c r="R32" s="114"/>
+      <c r="S32" s="114"/>
+      <c r="T32" s="114"/>
+      <c r="U32" s="115"/>
+      <c r="V32" s="59">
+        <f>SUM(V10:V30,0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A33" s="24">
+      <c r="A33" s="22">
         <v>23</v>
       </c>
       <c r="B33" s="75"/>
-      <c r="C33" s="113"/>
-      <c r="D33" s="113"/>
+      <c r="C33" s="108"/>
+      <c r="D33" s="108"/>
       <c r="E33" s="76"/>
       <c r="F33" s="75"/>
       <c r="G33" s="76"/>
       <c r="H33" s="75"/>
       <c r="I33" s="76"/>
       <c r="J33" s="75"/>
-      <c r="K33" s="113"/>
-      <c r="L33" s="113"/>
+      <c r="K33" s="108"/>
+      <c r="L33" s="108"/>
       <c r="M33" s="76"/>
       <c r="N33" s="75"/>
       <c r="O33" s="76"/>
-      <c r="Q33" s="34"/>
-      <c r="R33" s="34"/>
-      <c r="S33" s="35"/>
-      <c r="T33" s="35"/>
-      <c r="U33" s="35"/>
-      <c r="V33" s="36"/>
+      <c r="Q33" s="27"/>
+      <c r="R33" s="27"/>
+      <c r="S33" s="28"/>
+      <c r="T33" s="28"/>
+      <c r="U33" s="28"/>
+      <c r="V33" s="29"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A34" s="24">
+      <c r="A34" s="22">
         <v>24</v>
       </c>
       <c r="B34" s="75"/>
-      <c r="C34" s="113"/>
-      <c r="D34" s="113"/>
+      <c r="C34" s="108"/>
+      <c r="D34" s="108"/>
       <c r="E34" s="76"/>
       <c r="F34" s="75"/>
       <c r="G34" s="76"/>
       <c r="H34" s="75"/>
       <c r="I34" s="76"/>
       <c r="J34" s="75"/>
-      <c r="K34" s="113"/>
-      <c r="L34" s="113"/>
+      <c r="K34" s="108"/>
+      <c r="L34" s="108"/>
       <c r="M34" s="76"/>
       <c r="N34" s="75"/>
       <c r="O34" s="76"/>
-      <c r="Q34" s="34"/>
-      <c r="R34" s="34"/>
-      <c r="S34" s="35"/>
-      <c r="T34" s="35"/>
-      <c r="U34" s="35"/>
-      <c r="V34" s="36"/>
+      <c r="Q34" s="27"/>
+      <c r="R34" s="27"/>
+      <c r="S34" s="28"/>
+      <c r="T34" s="28"/>
+      <c r="U34" s="28"/>
+      <c r="V34" s="29"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A35" s="24">
+      <c r="A35" s="22">
         <v>25</v>
       </c>
       <c r="B35" s="75"/>
-      <c r="C35" s="113"/>
-      <c r="D35" s="113"/>
+      <c r="C35" s="108"/>
+      <c r="D35" s="108"/>
       <c r="E35" s="76"/>
       <c r="F35" s="75"/>
       <c r="G35" s="76"/>
       <c r="H35" s="75"/>
       <c r="I35" s="76"/>
       <c r="J35" s="75"/>
-      <c r="K35" s="113"/>
-      <c r="L35" s="113"/>
+      <c r="K35" s="108"/>
+      <c r="L35" s="108"/>
       <c r="M35" s="76"/>
       <c r="N35" s="75"/>
       <c r="O35" s="76"/>
-      <c r="Q35" s="34"/>
-      <c r="R35" s="34"/>
-      <c r="S35" s="35"/>
-      <c r="T35" s="35"/>
-      <c r="U35" s="35"/>
-      <c r="V35" s="36"/>
+      <c r="Q35" s="27"/>
+      <c r="R35" s="27"/>
+      <c r="S35" s="28"/>
+      <c r="T35" s="28"/>
+      <c r="U35" s="28"/>
+      <c r="V35" s="29"/>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A36" s="24">
+      <c r="A36" s="22">
         <v>26</v>
       </c>
       <c r="B36" s="75"/>
-      <c r="C36" s="113"/>
-      <c r="D36" s="113"/>
+      <c r="C36" s="108"/>
+      <c r="D36" s="108"/>
       <c r="E36" s="76"/>
       <c r="F36" s="75"/>
       <c r="G36" s="76"/>
       <c r="H36" s="75"/>
       <c r="I36" s="76"/>
       <c r="J36" s="75"/>
-      <c r="K36" s="113"/>
-      <c r="L36" s="113"/>
+      <c r="K36" s="108"/>
+      <c r="L36" s="108"/>
       <c r="M36" s="76"/>
       <c r="N36" s="75"/>
       <c r="O36" s="76"/>
-      <c r="Q36" s="34"/>
-      <c r="R36" s="34"/>
-      <c r="S36" s="35"/>
-      <c r="T36" s="35"/>
-      <c r="U36" s="35"/>
-      <c r="V36" s="36"/>
+      <c r="Q36" s="27"/>
+      <c r="R36" s="27"/>
+      <c r="S36" s="28"/>
+      <c r="T36" s="28"/>
+      <c r="U36" s="28"/>
+      <c r="V36" s="29"/>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A37" s="24">
+      <c r="A37" s="22">
         <v>27</v>
       </c>
       <c r="B37" s="75"/>
-      <c r="C37" s="113"/>
-      <c r="D37" s="113"/>
+      <c r="C37" s="108"/>
+      <c r="D37" s="108"/>
       <c r="E37" s="76"/>
       <c r="F37" s="75"/>
       <c r="G37" s="76"/>
       <c r="H37" s="75"/>
       <c r="I37" s="76"/>
       <c r="J37" s="75"/>
-      <c r="K37" s="113"/>
-      <c r="L37" s="113"/>
+      <c r="K37" s="108"/>
+      <c r="L37" s="108"/>
       <c r="M37" s="76"/>
       <c r="N37" s="75"/>
       <c r="O37" s="76"/>
-      <c r="Q37" s="37"/>
-      <c r="R37" s="37"/>
-      <c r="S37" s="37"/>
-      <c r="T37" s="36"/>
-      <c r="U37" s="36"/>
+      <c r="Q37" s="30"/>
+      <c r="R37" s="30"/>
+      <c r="S37" s="30"/>
+      <c r="T37" s="29"/>
+      <c r="U37" s="29"/>
     </row>
     <row r="38" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="24">
+      <c r="A38" s="22">
         <v>28</v>
       </c>
       <c r="B38" s="75"/>
-      <c r="C38" s="113"/>
-      <c r="D38" s="113"/>
+      <c r="C38" s="108"/>
+      <c r="D38" s="108"/>
       <c r="E38" s="76"/>
       <c r="F38" s="75"/>
       <c r="G38" s="76"/>
       <c r="H38" s="75"/>
       <c r="I38" s="76"/>
       <c r="J38" s="75"/>
-      <c r="K38" s="113"/>
-      <c r="L38" s="113"/>
+      <c r="K38" s="108"/>
+      <c r="L38" s="108"/>
       <c r="M38" s="76"/>
       <c r="N38" s="75"/>
       <c r="O38" s="76"/>
-      <c r="P38" s="38"/>
-      <c r="Q38" s="39"/>
-      <c r="R38" s="12"/>
-      <c r="S38" s="12"/>
-      <c r="T38" s="12"/>
-      <c r="U38" s="12"/>
+      <c r="P38" s="31"/>
+      <c r="Q38" s="32"/>
+      <c r="R38" s="11"/>
+      <c r="S38" s="11"/>
+      <c r="T38" s="11"/>
+      <c r="U38" s="11"/>
     </row>
     <row r="39" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="38"/>
-      <c r="R39" s="114"/>
-      <c r="S39" s="114"/>
-      <c r="T39" s="40"/>
-      <c r="U39" s="40"/>
+      <c r="A39" s="31"/>
+      <c r="R39" s="109"/>
+      <c r="S39" s="109"/>
+      <c r="T39" s="33"/>
+      <c r="U39" s="33"/>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A40" s="99" t="s">
+      <c r="A40" s="95" t="s">
         <v>68</v>
       </c>
-      <c r="B40" s="100"/>
-      <c r="C40" s="100"/>
-      <c r="D40" s="100"/>
-      <c r="E40" s="100"/>
-      <c r="F40" s="100"/>
-      <c r="G40" s="100"/>
-      <c r="H40" s="100"/>
-      <c r="I40" s="101"/>
-      <c r="J40" s="102" t="s">
+      <c r="B40" s="96"/>
+      <c r="C40" s="96"/>
+      <c r="D40" s="96"/>
+      <c r="E40" s="96"/>
+      <c r="F40" s="96"/>
+      <c r="G40" s="96"/>
+      <c r="H40" s="96"/>
+      <c r="I40" s="97"/>
+      <c r="J40" s="98" t="s">
         <v>69</v>
       </c>
-      <c r="K40" s="103"/>
-      <c r="L40" s="103"/>
-      <c r="M40" s="103"/>
-      <c r="N40" s="103"/>
-      <c r="O40" s="103"/>
-      <c r="P40" s="103"/>
-      <c r="Q40" s="103"/>
-      <c r="R40" s="103"/>
-      <c r="S40" s="103"/>
-      <c r="T40" s="103"/>
-      <c r="U40" s="103"/>
-      <c r="V40" s="104"/>
+      <c r="K40" s="99"/>
+      <c r="L40" s="99"/>
+      <c r="M40" s="99"/>
+      <c r="N40" s="99"/>
+      <c r="O40" s="99"/>
+      <c r="P40" s="99"/>
+      <c r="Q40" s="99"/>
+      <c r="R40" s="99"/>
+      <c r="S40" s="99"/>
+      <c r="T40" s="99"/>
+      <c r="U40" s="99"/>
+      <c r="V40" s="100"/>
       <c r="W40" s="1"/>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A41" s="41" t="s">
+      <c r="A41" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="B41" s="42"/>
-      <c r="C41" s="42"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="43" t="s">
+      <c r="B41" s="35"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="F41" s="105"/>
-      <c r="G41" s="105"/>
-      <c r="H41" s="105"/>
-      <c r="I41" s="106"/>
-      <c r="J41" s="107" t="s">
+      <c r="F41" s="101"/>
+      <c r="G41" s="101"/>
+      <c r="H41" s="101"/>
+      <c r="I41" s="81"/>
+      <c r="J41" s="102" t="s">
         <v>72</v>
       </c>
-      <c r="K41" s="108"/>
-      <c r="L41" s="108"/>
-      <c r="M41" s="108"/>
-      <c r="N41" s="109" t="s">
+      <c r="K41" s="103"/>
+      <c r="L41" s="103"/>
+      <c r="M41" s="103"/>
+      <c r="N41" s="104" t="s">
         <v>73</v>
       </c>
-      <c r="O41" s="109"/>
-      <c r="P41" s="110" t="s">
+      <c r="O41" s="104"/>
+      <c r="P41" s="105" t="s">
         <v>74</v>
       </c>
-      <c r="Q41" s="111"/>
-      <c r="R41" s="111"/>
-      <c r="S41" s="112"/>
-      <c r="T41" s="44" t="s">
+      <c r="Q41" s="106"/>
+      <c r="R41" s="106"/>
+      <c r="S41" s="107"/>
+      <c r="T41" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="U41" s="110" t="s">
+      <c r="U41" s="105" t="s">
         <v>76</v>
       </c>
-      <c r="V41" s="111"/>
-      <c r="W41" s="45"/>
+      <c r="V41" s="106"/>
+      <c r="W41" s="38"/>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A42" s="41" t="s">
+      <c r="A42" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="B42" s="42"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
-      <c r="E42" s="43" t="s">
+      <c r="B42" s="35"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
+      <c r="E42" s="36" t="s">
         <v>71</v>
       </c>
       <c r="F42" s="65"/>
       <c r="G42" s="65"/>
       <c r="H42" s="65"/>
       <c r="I42" s="86"/>
-      <c r="J42" s="46" t="s">
+      <c r="J42" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="K42" s="46"/>
-      <c r="L42" s="46"/>
-      <c r="M42" s="47"/>
-      <c r="N42" s="87"/>
+      <c r="K42" s="39"/>
+      <c r="L42" s="39"/>
+      <c r="M42" s="40"/>
+      <c r="N42" s="76"/>
       <c r="O42" s="74"/>
       <c r="P42" s="74"/>
       <c r="Q42" s="74"/>
       <c r="R42" s="74"/>
       <c r="S42" s="74"/>
-      <c r="T42" s="48"/>
+      <c r="T42" s="56"/>
       <c r="U42" s="75"/>
       <c r="V42" s="76"/>
       <c r="W42" s="1"/>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A43" s="88" t="s">
+      <c r="A43" s="87" t="s">
         <v>78</v>
       </c>
-      <c r="B43" s="89"/>
-      <c r="C43" s="89"/>
-      <c r="D43" s="42"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="90"/>
-      <c r="G43" s="90"/>
-      <c r="H43" s="90"/>
-      <c r="I43" s="91"/>
-      <c r="J43" s="92" t="s">
+      <c r="B43" s="88"/>
+      <c r="C43" s="88"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="36"/>
+      <c r="F43" s="65"/>
+      <c r="G43" s="65"/>
+      <c r="H43" s="65"/>
+      <c r="I43" s="86"/>
+      <c r="J43" s="89" t="s">
         <v>77</v>
       </c>
-      <c r="K43" s="93"/>
-      <c r="L43" s="93"/>
-      <c r="M43" s="94"/>
-      <c r="N43" s="87"/>
+      <c r="K43" s="90"/>
+      <c r="L43" s="90"/>
+      <c r="M43" s="91"/>
+      <c r="N43" s="76"/>
       <c r="O43" s="74"/>
       <c r="P43" s="74"/>
       <c r="Q43" s="74"/>
       <c r="R43" s="74"/>
       <c r="S43" s="74"/>
-      <c r="T43" s="98"/>
+      <c r="T43" s="74"/>
       <c r="U43" s="80"/>
       <c r="V43" s="81"/>
       <c r="W43" s="1"/>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A44" s="88"/>
-      <c r="B44" s="89"/>
-      <c r="C44" s="89"/>
+      <c r="A44" s="87"/>
+      <c r="B44" s="88"/>
+      <c r="C44" s="88"/>
       <c r="D44" s="1"/>
-      <c r="E44" s="43" t="s">
+      <c r="E44" s="36" t="s">
         <v>71</v>
       </c>
       <c r="F44" s="84"/>
       <c r="G44" s="84"/>
       <c r="H44" s="84"/>
       <c r="I44" s="85"/>
-      <c r="J44" s="95"/>
-      <c r="K44" s="96"/>
-      <c r="L44" s="96"/>
-      <c r="M44" s="97"/>
-      <c r="N44" s="87"/>
+      <c r="J44" s="92"/>
+      <c r="K44" s="93"/>
+      <c r="L44" s="93"/>
+      <c r="M44" s="94"/>
+      <c r="N44" s="76"/>
       <c r="O44" s="74"/>
       <c r="P44" s="74"/>
       <c r="Q44" s="74"/>
       <c r="R44" s="74"/>
       <c r="S44" s="74"/>
-      <c r="T44" s="98"/>
+      <c r="T44" s="74"/>
       <c r="U44" s="82"/>
       <c r="V44" s="83"/>
       <c r="W44" s="1"/>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A45" s="49"/>
+      <c r="A45" s="41"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -2897,17 +2884,17 @@
       <c r="Q45" s="74"/>
       <c r="R45" s="74"/>
       <c r="S45" s="74"/>
-      <c r="T45" s="48"/>
+      <c r="T45" s="56"/>
       <c r="U45" s="75"/>
       <c r="V45" s="76"/>
       <c r="W45" s="1"/>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A46" s="50"/>
-      <c r="B46" s="51"/>
-      <c r="C46" s="51"/>
-      <c r="D46" s="51"/>
-      <c r="E46" s="51"/>
+      <c r="A46" s="42"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="43"/>
+      <c r="E46" s="43"/>
       <c r="F46" s="68"/>
       <c r="G46" s="68"/>
       <c r="H46" s="68"/>
@@ -2924,7 +2911,7 @@
       <c r="Q46" s="74"/>
       <c r="R46" s="74"/>
       <c r="S46" s="74"/>
-      <c r="T46" s="48"/>
+      <c r="T46" s="56"/>
       <c r="U46" s="75"/>
       <c r="V46" s="76"/>
       <c r="W46" s="1"/>
@@ -2993,7 +2980,7 @@
       <c r="I49" s="67"/>
       <c r="J49" s="67"/>
       <c r="K49" s="67"/>
-      <c r="L49" s="52"/>
+      <c r="L49" s="44"/>
       <c r="M49" s="67" t="s">
         <v>83</v>
       </c>
@@ -3008,37 +2995,37 @@
       <c r="V49" s="67"/>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A50" s="53"/>
-      <c r="B50" s="54"/>
-      <c r="C50" s="54"/>
-      <c r="D50" s="54"/>
-      <c r="E50" s="54"/>
-      <c r="F50" s="54"/>
-      <c r="G50" s="54"/>
-      <c r="H50" s="54"/>
-      <c r="I50" s="54"/>
-      <c r="J50" s="54"/>
-      <c r="K50" s="54"/>
-      <c r="L50" s="55"/>
-      <c r="M50" s="53"/>
-      <c r="N50" s="54"/>
-      <c r="O50" s="54"/>
-      <c r="P50" s="54"/>
-      <c r="Q50" s="54"/>
-      <c r="R50" s="54"/>
-      <c r="S50" s="54"/>
-      <c r="T50" s="54"/>
-      <c r="U50" s="54"/>
-      <c r="V50" s="56"/>
+      <c r="A50" s="45"/>
+      <c r="B50" s="46"/>
+      <c r="C50" s="46"/>
+      <c r="D50" s="46"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="46"/>
+      <c r="G50" s="46"/>
+      <c r="H50" s="46"/>
+      <c r="I50" s="46"/>
+      <c r="J50" s="46"/>
+      <c r="K50" s="46"/>
+      <c r="L50" s="47"/>
+      <c r="M50" s="45"/>
+      <c r="N50" s="46"/>
+      <c r="O50" s="46"/>
+      <c r="P50" s="46"/>
+      <c r="Q50" s="46"/>
+      <c r="R50" s="46"/>
+      <c r="S50" s="46"/>
+      <c r="T50" s="46"/>
+      <c r="U50" s="46"/>
+      <c r="V50" s="48"/>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A51" s="41" t="s">
+      <c r="A51" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="B51" s="42"/>
-      <c r="C51" s="42"/>
-      <c r="D51" s="42"/>
-      <c r="E51" s="43" t="s">
+      <c r="B51" s="35"/>
+      <c r="C51" s="35"/>
+      <c r="D51" s="35"/>
+      <c r="E51" s="36" t="s">
         <v>71</v>
       </c>
       <c r="F51" s="65"/>
@@ -3047,13 +3034,13 @@
       <c r="I51" s="65"/>
       <c r="J51" s="65"/>
       <c r="K51" s="65"/>
-      <c r="L51" s="57"/>
-      <c r="M51" s="41" t="s">
+      <c r="L51" s="49"/>
+      <c r="M51" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="N51" s="42"/>
-      <c r="O51" s="42"/>
-      <c r="P51" s="42" t="s">
+      <c r="N51" s="35"/>
+      <c r="O51" s="35"/>
+      <c r="P51" s="35" t="s">
         <v>71</v>
       </c>
       <c r="Q51" s="65"/>
@@ -3061,16 +3048,16 @@
       <c r="S51" s="65"/>
       <c r="T51" s="65"/>
       <c r="U51" s="65"/>
-      <c r="V51" s="56"/>
+      <c r="V51" s="48"/>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A52" s="41" t="s">
+      <c r="A52" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="B52" s="42"/>
-      <c r="C52" s="42"/>
-      <c r="D52" s="42"/>
-      <c r="E52" s="42" t="s">
+      <c r="B52" s="35"/>
+      <c r="C52" s="35"/>
+      <c r="D52" s="35"/>
+      <c r="E52" s="35" t="s">
         <v>71</v>
       </c>
       <c r="F52" s="65"/>
@@ -3079,12 +3066,12 @@
       <c r="I52" s="65"/>
       <c r="J52" s="65"/>
       <c r="K52" s="65"/>
-      <c r="L52" s="58"/>
-      <c r="M52" s="41" t="s">
+      <c r="L52" s="50"/>
+      <c r="M52" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="O52" s="42"/>
-      <c r="P52" s="42" t="s">
+      <c r="O52" s="35"/>
+      <c r="P52" s="35" t="s">
         <v>71</v>
       </c>
       <c r="Q52" s="65"/>
@@ -3092,16 +3079,16 @@
       <c r="S52" s="65"/>
       <c r="T52" s="65"/>
       <c r="U52" s="65"/>
-      <c r="V52" s="59"/>
+      <c r="V52" s="57"/>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A53" s="41" t="s">
+      <c r="A53" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="B53" s="42"/>
-      <c r="C53" s="42"/>
-      <c r="D53" s="42"/>
-      <c r="E53" s="42" t="s">
+      <c r="B53" s="35"/>
+      <c r="C53" s="35"/>
+      <c r="D53" s="35"/>
+      <c r="E53" s="35" t="s">
         <v>71</v>
       </c>
       <c r="F53" s="65"/>
@@ -3110,12 +3097,12 @@
       <c r="I53" s="65"/>
       <c r="J53" s="65"/>
       <c r="K53" s="65"/>
-      <c r="L53" s="58"/>
-      <c r="M53" s="41" t="s">
+      <c r="L53" s="50"/>
+      <c r="M53" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="O53" s="42"/>
-      <c r="P53" s="42" t="s">
+      <c r="O53" s="35"/>
+      <c r="P53" s="35" t="s">
         <v>71</v>
       </c>
       <c r="Q53" s="65"/>
@@ -3126,13 +3113,13 @@
       <c r="V53" s="60"/>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A54" s="61" t="s">
+      <c r="A54" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="B54" s="62"/>
-      <c r="C54" s="62"/>
-      <c r="D54" s="62"/>
-      <c r="E54" s="62" t="s">
+      <c r="B54" s="52"/>
+      <c r="C54" s="52"/>
+      <c r="D54" s="52"/>
+      <c r="E54" s="52" t="s">
         <v>71</v>
       </c>
       <c r="F54" s="66"/>
@@ -3141,13 +3128,13 @@
       <c r="I54" s="66"/>
       <c r="J54" s="66"/>
       <c r="K54" s="66"/>
-      <c r="L54" s="63"/>
-      <c r="M54" s="61" t="s">
+      <c r="L54" s="53"/>
+      <c r="M54" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="N54" s="62"/>
-      <c r="O54" s="62"/>
-      <c r="P54" s="62" t="s">
+      <c r="N54" s="52"/>
+      <c r="O54" s="52"/>
+      <c r="P54" s="52" t="s">
         <v>71</v>
       </c>
       <c r="Q54" s="66"/>
@@ -3155,11 +3142,10 @@
       <c r="S54" s="66"/>
       <c r="T54" s="66"/>
       <c r="U54" s="66"/>
-      <c r="V54" s="64"/>
+      <c r="V54" s="61"/>
     </row>
   </sheetData>
-  <mergeCells count="205">
-    <mergeCell ref="Q32:U32"/>
+  <mergeCells count="206">
     <mergeCell ref="S30:U30"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:E10"/>
@@ -3257,11 +3243,6 @@
     <mergeCell ref="J25:M25"/>
     <mergeCell ref="N25:O25"/>
     <mergeCell ref="Q25:Q26"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:M29"/>
-    <mergeCell ref="N29:O29"/>
     <mergeCell ref="S29:U29"/>
     <mergeCell ref="R27:R28"/>
     <mergeCell ref="S27:U28"/>
@@ -3277,16 +3258,16 @@
     <mergeCell ref="J27:M27"/>
     <mergeCell ref="N27:O27"/>
     <mergeCell ref="Q27:Q28"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="J31:M31"/>
-    <mergeCell ref="N31:O31"/>
     <mergeCell ref="B30:E30"/>
     <mergeCell ref="F30:G30"/>
     <mergeCell ref="H30:I30"/>
     <mergeCell ref="J30:M30"/>
     <mergeCell ref="N30:O30"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:M29"/>
+    <mergeCell ref="N29:O29"/>
     <mergeCell ref="S31:U31"/>
     <mergeCell ref="B32:E32"/>
     <mergeCell ref="F32:G32"/>
@@ -3298,6 +3279,12 @@
     <mergeCell ref="H33:I33"/>
     <mergeCell ref="J33:M33"/>
     <mergeCell ref="N33:O33"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="J31:M31"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="Q32:U32"/>
     <mergeCell ref="B34:E34"/>
     <mergeCell ref="F34:G34"/>
     <mergeCell ref="H34:I34"/>
@@ -3341,6 +3328,17 @@
     <mergeCell ref="N43:O44"/>
     <mergeCell ref="P43:S44"/>
     <mergeCell ref="T43:T44"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="F53:K53"/>
+    <mergeCell ref="Q53:U53"/>
+    <mergeCell ref="F54:K54"/>
+    <mergeCell ref="Q54:U54"/>
+    <mergeCell ref="A49:K49"/>
+    <mergeCell ref="M49:V49"/>
+    <mergeCell ref="F51:K51"/>
+    <mergeCell ref="Q51:U51"/>
+    <mergeCell ref="F52:K52"/>
+    <mergeCell ref="Q52:U52"/>
     <mergeCell ref="F46:I46"/>
     <mergeCell ref="J46:M46"/>
     <mergeCell ref="N46:O46"/>
@@ -3354,16 +3352,6 @@
     <mergeCell ref="N45:O45"/>
     <mergeCell ref="P45:S45"/>
     <mergeCell ref="U45:V45"/>
-    <mergeCell ref="F53:K53"/>
-    <mergeCell ref="Q53:U53"/>
-    <mergeCell ref="F54:K54"/>
-    <mergeCell ref="Q54:U54"/>
-    <mergeCell ref="A49:K49"/>
-    <mergeCell ref="M49:V49"/>
-    <mergeCell ref="F51:K51"/>
-    <mergeCell ref="Q51:U51"/>
-    <mergeCell ref="F52:K52"/>
-    <mergeCell ref="Q52:U52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
excell ok until step 3
</commit_message>
<xml_diff>
--- a/formatexcel.xlsx
+++ b/formatexcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\FYP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE70D25-79EE-4561-A7DB-DDFF72AC113A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395368FD-3C4B-460F-81E7-0AE5F1416E36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{21832C7A-FE32-4B93-8F16-7397E18D770D}"/>
   </bookViews>
@@ -1162,138 +1162,92 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>586154</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>162977</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>262</xdr:colOff>
+      <xdr:colOff>158261</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>25231</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Rectangle 2">
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8727E25C-542C-4883-A230-2C2FA1C48665}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5880FE6E-6478-4858-BD4E-A461BF24C05F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6280785" y="910590"/>
-          <a:ext cx="333637" cy="171450"/>
+          <a:off x="6283569" y="1141854"/>
+          <a:ext cx="486507" cy="243254"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
       </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="ms-MY" sz="1100">
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>384077</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>13774</xdr:rowOff>
+      <xdr:colOff>234461</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>162977</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>720968</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>25231</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Rectangle 4">
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2C449C0-19D5-401D-A732-5C521B965134}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{623535B4-7531-43B6-BB69-F0DF5CD31DC7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7347585" y="1174359"/>
-          <a:ext cx="348615" cy="185518"/>
+          <a:off x="7274169" y="1141854"/>
+          <a:ext cx="486507" cy="243254"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
       </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="ms-MY" sz="1100">
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1598,21 +1552,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75980BA0-2244-437B-AE4D-E57234A9F6AA}">
   <dimension ref="A1:Y54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="V32" sqref="V32"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52:K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="4.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="7" style="2" customWidth="1"/>
     <col min="4" max="4" width="0.6640625" style="2" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="1.109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="2.88671875" style="2" customWidth="1"/>
     <col min="7" max="7" width="2.5546875" style="2" customWidth="1"/>
     <col min="8" max="8" width="5.33203125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="25.21875" style="2" customWidth="1"/>
     <col min="10" max="10" width="4.33203125" style="2" customWidth="1"/>
     <col min="11" max="11" width="5.44140625" style="2" customWidth="1"/>
     <col min="12" max="12" width="0.6640625" style="2" customWidth="1"/>
@@ -1624,7 +1578,7 @@
     <col min="18" max="18" width="6" style="2" customWidth="1"/>
     <col min="19" max="19" width="3.5546875" style="2" customWidth="1"/>
     <col min="20" max="20" width="13.33203125" style="2" customWidth="1"/>
-    <col min="21" max="21" width="5.109375" style="2" customWidth="1"/>
+    <col min="21" max="21" width="6.21875" style="2" customWidth="1"/>
     <col min="22" max="22" width="10.6640625" style="2" customWidth="1"/>
     <col min="23" max="23" width="7.6640625" style="2" customWidth="1"/>
   </cols>

</xml_diff>